<commit_message>
Octree C++ version beta
</commit_message>
<xml_diff>
--- a/doc/spheres/spheres-time.xlsx
+++ b/doc/spheres/spheres-time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Spheres</t>
   </si>
@@ -66,19 +66,34 @@
     <t>Octree level</t>
   </si>
   <si>
-    <t>Time 1</t>
+    <t>AVG collision checks (M)</t>
   </si>
   <si>
-    <t>Time 2</t>
+    <t>JS Time 1</t>
   </si>
   <si>
-    <t>Time 3</t>
+    <t>JS Time 2</t>
   </si>
   <si>
-    <t>AVG Time</t>
+    <t>JS Time 3</t>
   </si>
   <si>
-    <t>AVG collision checks (M)</t>
+    <t>JS AVG Time</t>
+  </si>
+  <si>
+    <t>C++ Time 1</t>
+  </si>
+  <si>
+    <t>C++ Time 2</t>
+  </si>
+  <si>
+    <t>C++ Time 3</t>
+  </si>
+  <si>
+    <t>C++ AVG Time</t>
+  </si>
+  <si>
+    <t>C++ % faster</t>
   </si>
 </sst>
 </file>
@@ -173,7 +188,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -386,11 +400,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39018880"/>
-        <c:axId val="39020416"/>
+        <c:axId val="94003200"/>
+        <c:axId val="94004736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39018880"/>
+        <c:axId val="94003200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -400,7 +414,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39020416"/>
+        <c:crossAx val="94004736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -408,7 +422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39020416"/>
+        <c:axId val="94004736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,14 +445,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39018880"/>
+        <c:crossAx val="94003200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -496,7 +509,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -709,11 +721,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39190912"/>
-        <c:axId val="39192448"/>
+        <c:axId val="42532864"/>
+        <c:axId val="42534400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39190912"/>
+        <c:axId val="42532864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -723,7 +735,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39192448"/>
+        <c:crossAx val="42534400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -731,7 +743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39192448"/>
+        <c:axId val="42534400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -756,14 +768,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39190912"/>
+        <c:crossAx val="42532864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -847,7 +858,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG Time</c:v>
+                  <c:v>JS AVG Time</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -890,6 +901,64 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>19.50266666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz2!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++ AVG Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Arkusz2!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5550000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6483333333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1323333333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58233333333333326</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51066666666666671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4616666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7006666666666668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.7596666666666669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.302666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,11 +975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53473664"/>
-        <c:axId val="53475200"/>
+        <c:axId val="42589568"/>
+        <c:axId val="42591360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53473664"/>
+        <c:axId val="42589568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +988,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53475200"/>
+        <c:crossAx val="42591360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -927,7 +996,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53475200"/>
+        <c:axId val="42591360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +1007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53473664"/>
+        <c:crossAx val="42589568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1008,7 +1077,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Arkusz2!$A$6</c:f>
+              <c:f>Arkusz2!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1022,7 +1091,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Arkusz2!$B$6:$K$6</c:f>
+              <c:f>Arkusz2!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1071,11 +1140,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="53892224"/>
-        <c:axId val="53893760"/>
+        <c:axId val="42611456"/>
+        <c:axId val="42612992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53892224"/>
+        <c:axId val="42611456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1153,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53893760"/>
+        <c:crossAx val="42612992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1092,7 +1161,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53893760"/>
+        <c:axId val="42612992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1172,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53892224"/>
+        <c:crossAx val="42611456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,15 +1261,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1222,15 +1291,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2148,10 +2217,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,7 +2266,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>3.71</v>
@@ -2232,7 +2301,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>3.6709999999999998</v>
@@ -2267,7 +2336,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>3.722</v>
@@ -2302,7 +2371,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <f>AVERAGE(B2:B4)</f>
@@ -2347,37 +2416,232 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6">
+        <v>2.5880000000000001</v>
+      </c>
+      <c r="C6">
+        <v>1.694</v>
+      </c>
+      <c r="D6">
+        <v>1.202</v>
+      </c>
+      <c r="E6">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.876</v>
+      </c>
+      <c r="H6">
+        <v>1.5569999999999999</v>
+      </c>
+      <c r="I6">
+        <v>2.74</v>
+      </c>
+      <c r="J6">
+        <v>5.8689999999999998</v>
+      </c>
+      <c r="K6">
+        <v>14.516999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>2.5329999999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.1020000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F7">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="G7">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="H7">
+        <v>1.421</v>
+      </c>
+      <c r="I7">
+        <v>2.6309999999999998</v>
+      </c>
+      <c r="J7">
+        <v>5.7469999999999999</v>
+      </c>
+      <c r="K7">
+        <v>14.205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>2.544</v>
+      </c>
+      <c r="C8">
+        <v>1.627</v>
+      </c>
+      <c r="D8">
+        <v>1.093</v>
+      </c>
+      <c r="E8">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="F8">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="H8">
+        <v>1.407</v>
+      </c>
+      <c r="I8">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="J8">
+        <v>5.6630000000000003</v>
+      </c>
+      <c r="K8">
+        <v>14.186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(B6:B8)</f>
+        <v>2.5550000000000002</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:K9" si="1">AVERAGE(C6:C8)</f>
+        <v>1.6483333333333334</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1.1323333333333334</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.58233333333333326</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.51066666666666671</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.4616666666666667</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>2.7006666666666668</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>5.7596666666666669</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>14.302666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
         <v>250</v>
       </c>
-      <c r="C6">
+      <c r="C10">
         <v>150</v>
       </c>
-      <c r="D6">
+      <c r="D10">
         <v>90</v>
       </c>
-      <c r="E6">
+      <c r="E10">
         <v>40</v>
       </c>
-      <c r="F6">
+      <c r="F10">
         <v>12</v>
       </c>
-      <c r="G6">
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="H6">
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="I6">
+      <c r="I10">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="J10">
         <v>9</v>
       </c>
-      <c r="K6">
+      <c r="K10">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2">
+        <f>B5/B9-1</f>
+        <v>0.44853228962818004</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ref="C11:K11" si="2">C5/C9-1</f>
+        <v>0.39453993933265918</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.31468943185163378</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.46708643388666293</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.63185378590078312</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.73145979703356745</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.79201824401368315</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.72685756603307827</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.46605706348747034</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.36356856530250781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>